<commit_message>
Redo name change to undo
</commit_message>
<xml_diff>
--- a/Excel files/slot.xlsx
+++ b/Excel files/slot.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SLOT</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -559,7 +559,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SLOT</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">

</xml_diff>

<commit_message>
undo and Save added
</commit_message>
<xml_diff>
--- a/Excel files/slot.xlsx
+++ b/Excel files/slot.xlsx
@@ -354,29 +354,24 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>8:00 - 8:50</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>9:00 - 9:50</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>10:00 - 10:50</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>11:00 - 11:50</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>12:00 - 12:50</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -413,7 +408,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>SLOT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -443,7 +438,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>SLOT</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -470,7 +465,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>SLOT</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -522,7 +517,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>SLOT</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -559,7 +554,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>SLOT</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -579,7 +574,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>SLOT</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -631,7 +626,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>SLOT</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">

</xml_diff>